<commit_message>
partial solutions for part b and c
</commit_message>
<xml_diff>
--- a/Lab1/Lab1.xlsx
+++ b/Lab1/Lab1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ENGO634\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E94FBE-A684-4344-B863-A74737DD958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E3412E-2FF5-4847-ACD5-DF92849E410D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11445" yWindow="2370" windowWidth="20835" windowHeight="15885" xr2:uid="{792B6195-0286-46E9-97B6-988B0F14CD54}"/>
+    <workbookView xWindow="-22035" yWindow="6255" windowWidth="20835" windowHeight="15885" xr2:uid="{792B6195-0286-46E9-97B6-988B0F14CD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93710F6A-4497-4138-9EB6-599565C0B4F3}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3</v>
       </c>
@@ -437,8 +437,17 @@
       <c r="C1">
         <v>1472</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>304</v>
+      </c>
+      <c r="F1">
+        <v>2546</v>
+      </c>
+      <c r="G1">
+        <v>5779</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -448,8 +457,17 @@
       <c r="C2">
         <v>10378</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>4544</v>
+      </c>
+      <c r="G2">
+        <v>17489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -460,7 +478,7 @@
         <v>19284</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -471,7 +489,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -482,7 +500,7 @@
         <v>19792</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -493,7 +511,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -504,7 +522,7 @@
         <v>10385</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -515,12 +533,12 @@
         <v>19291</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -531,7 +549,7 @@
         <v>11608</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>

</xml_diff>